<commit_message>
clean version of catalan-juvenile-recidivism data
</commit_message>
<xml_diff>
--- a/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-NaNs.xlsx
+++ b/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-NaNs.xlsx
@@ -755,7 +755,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>V12_n_criminal_record_cat</t>
+          <t>V12_n_criminal_record</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>V22_comission_date_of_main_crime</t>
+          <t>V22_main_crime_comission_date</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>V27_duration_of_program_cat</t>
+          <t>V27_program_duration_cat</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>V28_days_between_crime_and_program</t>
+          <t>V28_days_from_crime_to_program</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>V29_duration_of_program</t>
+          <t>V29_program_duration</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>V30_start_date_of_program</t>
+          <t>V30_program_start</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>V31_finish_date_of_program</t>
+          <t>V31_program_end</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -3065,7 +3065,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>V115_RECID2015_recid_bool</t>
+          <t>V115_RECID2015_recid</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>V132_RECID2013_recid_bool</t>
+          <t>V132_RECID2013_recid</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">

</xml_diff>

<commit_message>
omitting V14_comitted_crime from catalan data
</commit_message>
<xml_diff>
--- a/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-NaNs.xlsx
+++ b/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-NaNs.xlsx
@@ -839,7 +839,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>V16_violent_record</t>
+          <t>V16_violent_crime</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>V19_comitted_crime</t>
+          <t>V19_committed_crime</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">

</xml_diff>